<commit_message>
Slightly improved report preparation by adding new styles, added log4j and one test case
</commit_message>
<xml_diff>
--- a/src/test/java/resources/TestData.xlsx
+++ b/src/test/java/resources/TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Country</t>
   </si>
@@ -132,6 +132,30 @@
   </si>
   <si>
     <t>Company</t>
+  </si>
+  <si>
+    <t>Credit card holder name</t>
+  </si>
+  <si>
+    <t>Expiry date</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Arno</t>
+  </si>
+  <si>
+    <t>2028-02</t>
+  </si>
+  <si>
+    <t>2048-04</t>
+  </si>
+  <si>
+    <t>Abc</t>
+  </si>
+  <si>
+    <t>Abcd12</t>
   </si>
 </sst>
 </file>
@@ -176,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -185,6 +209,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -468,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,10 +512,10 @@
     <col min="9" max="9" width="19.88671875" customWidth="1"/>
     <col min="10" max="10" width="13.21875" customWidth="1"/>
     <col min="11" max="11" width="12.5546875" customWidth="1"/>
-    <col min="14" max="14" width="15.109375" customWidth="1"/>
+    <col min="14" max="16" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,13 +559,19 @@
         <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -581,8 +614,14 @@
       <c r="N2" s="1">
         <v>40000353535</v>
       </c>
+      <c r="O2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -626,35 +665,65 @@
         <v>40000353535</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="3"/>
+    <row r="4" spans="1:18" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed the project successfully
</commit_message>
<xml_diff>
--- a/src/test/java/resources/TestData.xlsx
+++ b/src/test/java/resources/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X085271\Downloads\automated-testing-master@a4715cf2524\Signup\src\test\java\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\Signup\src\test\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="70">
   <si>
     <t>Country</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Anderson</t>
   </si>
   <si>
-    <t>mike.andy@gmail.com</t>
-  </si>
-  <si>
     <t>Abcd1234</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>CH</t>
   </si>
   <si>
-    <t>4434ch</t>
-  </si>
-  <si>
     <t>Discovery</t>
   </si>
   <si>
@@ -146,9 +140,6 @@
     <t>Arno</t>
   </si>
   <si>
-    <t>2028-02</t>
-  </si>
-  <si>
     <t>2048-04</t>
   </si>
   <si>
@@ -156,6 +147,93 @@
   </si>
   <si>
     <t>Abcd12</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>3636rt</t>
+  </si>
+  <si>
+    <t>abc.def</t>
+  </si>
+  <si>
+    <t>Direct Debit</t>
+  </si>
+  <si>
+    <t>NL94BCNA0287125456</t>
+  </si>
+  <si>
+    <t>AB3432</t>
+  </si>
+  <si>
+    <t>IBAN</t>
+  </si>
+  <si>
+    <t>BIC</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Robin</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>abcd.zxeg@gmail.com</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>444444444444444</t>
+  </si>
+  <si>
+    <t>Maximus</t>
+  </si>
+  <si>
+    <t>2028-04</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>Expiry month</t>
+  </si>
+  <si>
+    <t>Expiry Year</t>
+  </si>
+  <si>
+    <t>788323394</t>
+  </si>
+  <si>
+    <t>SGSE343</t>
+  </si>
+  <si>
+    <t>3432RT</t>
+  </si>
+  <si>
+    <t>Credit card France</t>
+  </si>
+  <si>
+    <t>6824</t>
+  </si>
+  <si>
+    <t>johnny.andrew@gmail.com</t>
+  </si>
+  <si>
+    <t>788957394</t>
   </si>
 </sst>
 </file>
@@ -211,7 +289,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -495,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,10 +590,10 @@
     <col min="9" max="9" width="19.88671875" customWidth="1"/>
     <col min="10" max="10" width="13.21875" customWidth="1"/>
     <col min="11" max="11" width="12.5546875" customWidth="1"/>
-    <col min="14" max="16" width="15.109375" customWidth="1"/>
+    <col min="14" max="19" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -541,7 +619,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -559,27 +637,42 @@
         <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>15</v>
@@ -588,142 +681,359 @@
         <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" s="1">
         <v>49</v>
       </c>
-      <c r="J2" s="1">
-        <v>100000</v>
+      <c r="J2" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N2" s="4">
+        <v>40000353535</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>2028</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2" s="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1">
+        <v>33</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P3" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>2028</v>
+      </c>
+      <c r="S3" s="1">
+        <v>124</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="1">
+      <c r="U3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:23" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5">
+        <v>43</v>
+      </c>
+      <c r="J5" s="4">
+        <v>687768214</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="1">
+        <v>41</v>
+      </c>
+      <c r="J6" s="4">
+        <v>687768214</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="4">
         <v>40000353535</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>40</v>
+      <c r="T6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="7" spans="1:23" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="1">
+        <v>41</v>
+      </c>
+      <c r="J7" s="4">
+        <v>687768214</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="L7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="4">
+        <v>40000353535</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1">
         <v>41</v>
       </c>
-      <c r="J3" s="1">
-        <v>44444444</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="1">
-        <v>40000353535</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>24</v>
+      <c r="J8" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="F3" r:id="rId2"/>
     <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId4"/>
+    <hyperlink ref="F7" r:id="rId5"/>
+    <hyperlink ref="F8" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed unused library from dependencies
</commit_message>
<xml_diff>
--- a/src/test/java/resources/TestData.xlsx
+++ b/src/test/java/resources/TestData.xlsx
@@ -230,10 +230,10 @@
     <t>6824</t>
   </si>
   <si>
-    <t>johnny.andrew@gmail.com</t>
-  </si>
-  <si>
-    <t>788957394</t>
+    <t>jonny.andrew@gmail.com</t>
+  </si>
+  <si>
+    <t>788967494</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
   <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>